<commit_message>
adicionado banco de dados sqlite para armazenar os hashes
</commit_message>
<xml_diff>
--- a/cnpj.xlsx
+++ b/cnpj.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno.martins\Desktop\Automações\Sieg\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno.martins\Desktop\Sieg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A7F32C-8531-4584-B4BC-DD633A146C65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4E52AB-4DBD-44B4-8666-F7F99C966DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4050" yWindow="1110" windowWidth="15120" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
   <si>
     <t>CNPJ</t>
   </si>
@@ -115,6 +115,459 @@
   </si>
   <si>
     <t>48.620.694/0001-96</t>
+  </si>
+  <si>
+    <t>32.192.180/0001-47</t>
+  </si>
+  <si>
+    <t>01.803.861/0001-70</t>
+  </si>
+  <si>
+    <t>45.551.512/0001-84</t>
+  </si>
+  <si>
+    <t>12.407.089/0001-94</t>
+  </si>
+  <si>
+    <t>49.920.531/0001-91</t>
+  </si>
+  <si>
+    <t>10.251.103/0001-88</t>
+  </si>
+  <si>
+    <t>04.591.902/0001-09</t>
+  </si>
+  <si>
+    <t>20.330.514/0001-12</t>
+  </si>
+  <si>
+    <t>05.426.225/0001-28</t>
+  </si>
+  <si>
+    <t>24.080.055/0001-17</t>
+  </si>
+  <si>
+    <t>53.858.320/0001-43</t>
+  </si>
+  <si>
+    <t>37.812.627/0001-57</t>
+  </si>
+  <si>
+    <t>45.528.148/0001-31</t>
+  </si>
+  <si>
+    <t>08.493.672/0001-98</t>
+  </si>
+  <si>
+    <t>57.190.544/0001-80</t>
+  </si>
+  <si>
+    <t>64.958.663/0001-04</t>
+  </si>
+  <si>
+    <t>31.253.286/0001-40</t>
+  </si>
+  <si>
+    <t>02.361.748/0001-45</t>
+  </si>
+  <si>
+    <t>19.221.171/0001-79</t>
+  </si>
+  <si>
+    <t>14.441.136/0001-41</t>
+  </si>
+  <si>
+    <t>17.161.602/0001-23</t>
+  </si>
+  <si>
+    <t>41.539.045/0001-16</t>
+  </si>
+  <si>
+    <t>11.819.159/0001-59</t>
+  </si>
+  <si>
+    <t>48.620.694/0002-77</t>
+  </si>
+  <si>
+    <t>49.920.531/0002-72</t>
+  </si>
+  <si>
+    <t>26.899.221/0003-07</t>
+  </si>
+  <si>
+    <t>10.493.581/0003-66</t>
+  </si>
+  <si>
+    <t>48.620.694/0003-58</t>
+  </si>
+  <si>
+    <t>12.407.089/0002-75</t>
+  </si>
+  <si>
+    <t>49.920.531/0003-53</t>
+  </si>
+  <si>
+    <t>57.622.722/0002-86</t>
+  </si>
+  <si>
+    <t>12.407.089/0003-56</t>
+  </si>
+  <si>
+    <t>49.920.531/0004-34</t>
+  </si>
+  <si>
+    <t>04.253.313/0003-74</t>
+  </si>
+  <si>
+    <t>04.253.313/0004-55</t>
+  </si>
+  <si>
+    <t>46.905.296/0001-90</t>
+  </si>
+  <si>
+    <t>45.551.512/0002-65</t>
+  </si>
+  <si>
+    <t>37.438.812/0001-23</t>
+  </si>
+  <si>
+    <t>13.216.823/0001-09</t>
+  </si>
+  <si>
+    <t>64.059.009/0001-50</t>
+  </si>
+  <si>
+    <t>09.241.535/0001-29</t>
+  </si>
+  <si>
+    <t>74.625.369/0001-26</t>
+  </si>
+  <si>
+    <t>14.003.724/0001-01</t>
+  </si>
+  <si>
+    <t>30.922.463/0001-71</t>
+  </si>
+  <si>
+    <t>13.871.662/0001-89</t>
+  </si>
+  <si>
+    <t>72.815.350/0001-17</t>
+  </si>
+  <si>
+    <t>01.083.122/0001-51</t>
+  </si>
+  <si>
+    <t>27.324.473/0001-09</t>
+  </si>
+  <si>
+    <t>37.650.866/0001-58</t>
+  </si>
+  <si>
+    <t>47.734.947/0001-90</t>
+  </si>
+  <si>
+    <t>32.707.447/0001-91</t>
+  </si>
+  <si>
+    <t>04.253.313/0001-02</t>
+  </si>
+  <si>
+    <t>18.101.284/0001-78</t>
+  </si>
+  <si>
+    <t>57.622.722/0001-03</t>
+  </si>
+  <si>
+    <t>09.142.005/0001-23</t>
+  </si>
+  <si>
+    <t>20.533.990/0001-30</t>
+  </si>
+  <si>
+    <t>10.350.863/0001-42</t>
+  </si>
+  <si>
+    <t>07.595.849/0001-02</t>
+  </si>
+  <si>
+    <t>43.849.534/0001-08</t>
+  </si>
+  <si>
+    <t>55.807.715/0001-42</t>
+  </si>
+  <si>
+    <t>20.667.541/0001-85</t>
+  </si>
+  <si>
+    <t>09.578.248/0001-09</t>
+  </si>
+  <si>
+    <t>23.857.176/0001-60</t>
+  </si>
+  <si>
+    <t>15.503.556/0001-78</t>
+  </si>
+  <si>
+    <t>20.901.766/0001-54</t>
+  </si>
+  <si>
+    <t>09.284.051/0001-67</t>
+  </si>
+  <si>
+    <t>42.177.591/0001-17</t>
+  </si>
+  <si>
+    <t>29.022.776/0001-94</t>
+  </si>
+  <si>
+    <t>02.316.330/0001-16</t>
+  </si>
+  <si>
+    <t>45.481.709/0001-94</t>
+  </si>
+  <si>
+    <t>02.344.159/0001-59</t>
+  </si>
+  <si>
+    <t>13.452.799/0001-07</t>
+  </si>
+  <si>
+    <t>05.350.981/0001-10</t>
+  </si>
+  <si>
+    <t>11.688.117/0001-26</t>
+  </si>
+  <si>
+    <t>08.059.154/0001-60</t>
+  </si>
+  <si>
+    <t>43.188.402/0001-74</t>
+  </si>
+  <si>
+    <t>23.343.042/0001-20</t>
+  </si>
+  <si>
+    <t>57.092.912/0001-58</t>
+  </si>
+  <si>
+    <t>46.747.455/0001-76</t>
+  </si>
+  <si>
+    <t>09.240.049/0001-96</t>
+  </si>
+  <si>
+    <t>09.419.898/0001-01</t>
+  </si>
+  <si>
+    <t>19.726.627/0001-52</t>
+  </si>
+  <si>
+    <t>41.319.486/0001-02</t>
+  </si>
+  <si>
+    <t>48.461.953/0001-83</t>
+  </si>
+  <si>
+    <t>18.583.562/0001-70</t>
+  </si>
+  <si>
+    <t>21.508.579/0001-78</t>
+  </si>
+  <si>
+    <t>10.779.535/0001-66</t>
+  </si>
+  <si>
+    <t>52.100.416/0001-85</t>
+  </si>
+  <si>
+    <t>11.850.406/0001-80</t>
+  </si>
+  <si>
+    <t>18.933.521/0001-67</t>
+  </si>
+  <si>
+    <t>03.409.583/0001-05</t>
+  </si>
+  <si>
+    <t>38.311.265/0001-83</t>
+  </si>
+  <si>
+    <t>02.961.049/0001-36</t>
+  </si>
+  <si>
+    <t>20.072.176/0001-66</t>
+  </si>
+  <si>
+    <t>52.490.938/0001-30</t>
+  </si>
+  <si>
+    <t>55.121.844/0001-82</t>
+  </si>
+  <si>
+    <t>04.494.585/0001-02</t>
+  </si>
+  <si>
+    <t>44.734.994/0001-45</t>
+  </si>
+  <si>
+    <t>07.499.258/0001-23</t>
+  </si>
+  <si>
+    <t>50.830.820/0001-89</t>
+  </si>
+  <si>
+    <t>10.265.831/0001-49</t>
+  </si>
+  <si>
+    <t>05.667.946/0001-20</t>
+  </si>
+  <si>
+    <t>09.550.876/0001-86</t>
+  </si>
+  <si>
+    <t>01.706.432/0001-85</t>
+  </si>
+  <si>
+    <t>33.863.050/0001-51</t>
+  </si>
+  <si>
+    <t>33.579.158/0001-17</t>
+  </si>
+  <si>
+    <t>46.472.550/0001-04</t>
+  </si>
+  <si>
+    <t>43.849.399/0001-92</t>
+  </si>
+  <si>
+    <t>00.162.337/0001-03</t>
+  </si>
+  <si>
+    <t>17.630.452/0001-50</t>
+  </si>
+  <si>
+    <t>68.210.665/0001-63</t>
+  </si>
+  <si>
+    <t>47.192.621/0001-88</t>
+  </si>
+  <si>
+    <t>10.798.563/0001-20</t>
+  </si>
+  <si>
+    <t>30.353.141/0001-59</t>
+  </si>
+  <si>
+    <t>07.153.849/0001-44</t>
+  </si>
+  <si>
+    <t>96.682.067/0001-22</t>
+  </si>
+  <si>
+    <t>06.956.200/0001-07</t>
+  </si>
+  <si>
+    <t>27.547.731/0001-08</t>
+  </si>
+  <si>
+    <t>16.550.677/0001-33</t>
+  </si>
+  <si>
+    <t>11.024.035/0001-87</t>
+  </si>
+  <si>
+    <t>22.812.385/0001-24</t>
+  </si>
+  <si>
+    <t>35.794.193/0001-84</t>
+  </si>
+  <si>
+    <t>00.574.215/0001-16</t>
+  </si>
+  <si>
+    <t>39.814.432/0001-71</t>
+  </si>
+  <si>
+    <t>19.761.898/0001-49</t>
+  </si>
+  <si>
+    <t>52.314.002/0001-59</t>
+  </si>
+  <si>
+    <t>29.933.257/0001-88</t>
+  </si>
+  <si>
+    <t>24.635.002/0001-15</t>
+  </si>
+  <si>
+    <t>00.183.296/0001-23</t>
+  </si>
+  <si>
+    <t>39.465.176/0001-54</t>
+  </si>
+  <si>
+    <t>08.732.024/0001-47</t>
+  </si>
+  <si>
+    <t>26.899.221/0001-37</t>
+  </si>
+  <si>
+    <t>74.638.834/0001-63</t>
+  </si>
+  <si>
+    <t>52.845.435/0001-30</t>
+  </si>
+  <si>
+    <t>40.129.573/0001-34</t>
+  </si>
+  <si>
+    <t>44.361.705/0001-00</t>
+  </si>
+  <si>
+    <t>11.685.846/0001-29</t>
+  </si>
+  <si>
+    <t>05.650.012/0001-85</t>
+  </si>
+  <si>
+    <t>55.424.291/0001-37</t>
+  </si>
+  <si>
+    <t>14.975.895/0001-94</t>
+  </si>
+  <si>
+    <t>04.581.091/0001-57</t>
+  </si>
+  <si>
+    <t>02.458.761/0001-17</t>
+  </si>
+  <si>
+    <t>11.737.802/0001-03</t>
+  </si>
+  <si>
+    <t>51.307.276/0001-58</t>
+  </si>
+  <si>
+    <t>43.750.941/0001-55</t>
+  </si>
+  <si>
+    <t>54.898.865/0001-46</t>
+  </si>
+  <si>
+    <t>07.538.935/0001-75</t>
+  </si>
+  <si>
+    <t>19.956.967/0001-70</t>
+  </si>
+  <si>
+    <t>48.869.875/0001-50</t>
+  </si>
+  <si>
+    <t>31.532.172/0001-30</t>
+  </si>
+  <si>
+    <t>01.054.712/0001-56</t>
   </si>
 </sst>
 </file>
@@ -443,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A30"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,459 +1056,762 @@
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
+      <c r="A53" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
+      <c r="A55" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
+      <c r="A59" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
+      <c r="A63" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
+      <c r="A65" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
+      <c r="A66" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
+      <c r="A67" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
+      <c r="A69" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
+      <c r="A71" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
+      <c r="A72" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
+      <c r="A73" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
+      <c r="A74" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
+      <c r="A75" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
+      <c r="A77" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
+      <c r="A78" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
+      <c r="A79" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
+      <c r="A80" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
+      <c r="A81" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
+      <c r="A82" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
+      <c r="A83" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
+      <c r="A84" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
+      <c r="A85" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
+      <c r="A87" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
+      <c r="A88" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
+      <c r="A89" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
+      <c r="A90" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
+      <c r="A91" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
+      <c r="A92" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
+      <c r="A93" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
+      <c r="A94" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
+      <c r="A95" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
+      <c r="A96" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
+      <c r="A97" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
+      <c r="A98" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
+      <c r="A99" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
+      <c r="A100" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
+      <c r="A101" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
+      <c r="A102" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
+      <c r="A103" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
+      <c r="A104" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
+      <c r="A105" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
+      <c r="A106" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
+      <c r="A107" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
+      <c r="A108" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
+      <c r="A109" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
+      <c r="A110" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
+      <c r="A111" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
+      <c r="A112" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
+      <c r="A113" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
+      <c r="A114" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
+      <c r="A115" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
+      <c r="A116" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
+      <c r="A117" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
+      <c r="A118" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
+      <c r="A119" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
+      <c r="A120" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
+      <c r="A121" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
+      <c r="A122" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
+      <c r="A123" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
+      <c r="A124" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="1"/>
+      <c r="A125" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
+      <c r="A126" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="1"/>
+      <c r="A127" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="1"/>
+      <c r="A128" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="1"/>
+      <c r="A129" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="1"/>
+      <c r="A130" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="1"/>
+      <c r="A131" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="1"/>
+      <c r="A132" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="1"/>
+      <c r="A133" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="1"/>
+      <c r="A134" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="1"/>
+      <c r="A135" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="1"/>
+      <c r="A136" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
+      <c r="A137" s="1" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1"/>
+      <c r="A138" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="1"/>
+      <c r="A139" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="1"/>
+      <c r="A140" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="1"/>
+      <c r="A141" s="1" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="1"/>
+      <c r="A142" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="1"/>
+      <c r="A143" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="1"/>
+      <c r="A144" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="1"/>
+      <c r="A145" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="1"/>
+      <c r="A146" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="1"/>
+      <c r="A147" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="1"/>
+      <c r="A148" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="1"/>
+      <c r="A149" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="1"/>
+      <c r="A150" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="1"/>
+      <c r="A151" s="1" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="1"/>
+      <c r="A152" s="1" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="1"/>
+      <c r="A153" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="1"/>
+      <c r="A154" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="1"/>
+      <c r="A155" s="1" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="1"/>
+      <c r="A156" s="1" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="1"/>
+      <c r="A157" s="1" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="1"/>
+      <c r="A158" s="1" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="1"/>
+      <c r="A159" s="1" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="1"/>
+      <c r="A160" s="1" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="1"/>
+      <c r="A161" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="1"/>
+      <c r="A162" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="1"/>
+      <c r="A163" s="1" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="1"/>
+      <c r="A164" s="1" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="1"/>
+      <c r="A165" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="1"/>
+      <c r="A166" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="1"/>
+      <c r="A167" s="1" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="1"/>
+      <c r="A168" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="1"/>
+      <c r="A169" s="1" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="1"/>
+      <c r="A170" s="1" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="1"/>
+      <c r="A171" s="1" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="1"/>
+      <c r="A172" s="1" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="1"/>
+      <c r="A173" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="1"/>
+      <c r="A174" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="1"/>
+      <c r="A175" s="1" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="1"/>
+      <c r="A176" s="1" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="1"/>
+      <c r="A177" s="1" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="1"/>
+      <c r="A178" s="1" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="1"/>
+      <c r="A179" s="1" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="1"/>
+      <c r="A180" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="1"/>
+      <c r="A181" s="1" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
modificado verificações para download e salvamento
</commit_message>
<xml_diff>
--- a/cnpj.xlsx
+++ b/cnpj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno.martins\Desktop\Sieg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AF8936C-0ED9-494A-ACF5-E2745D7CEE6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35007D3-EBAA-4974-A02A-C3B9C37A80CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>CNPJ</t>
   </si>
@@ -33,7 +33,7 @@
     <t>05.574.628/0001-14</t>
   </si>
   <si>
-    <t>27.935.508/0001-38</t>
+    <t>27.988.301/0001-21</t>
   </si>
   <si>
     <t>43.492.777/0001-23</t>
@@ -48,19 +48,13 @@
     <t>22.726.051/0001-38</t>
   </si>
   <si>
+    <t>27.935.508/0001-38</t>
+  </si>
+  <si>
     <t>34.467.517/0001-07</t>
   </si>
   <si>
     <t>46.701.113/0001-15</t>
-  </si>
-  <si>
-    <t>28.860.597/0001-63</t>
-  </si>
-  <si>
-    <t>42.856.348/0001-25</t>
-  </si>
-  <si>
-    <t>11.023.210/0001-11</t>
   </si>
 </sst>
 </file>
@@ -390,7 +384,7 @@
   <dimension ref="A1:A181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -405,7 +399,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -435,28 +429,24 @@
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
     </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+    </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
+      <c r="A12" s="1"/>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>

</xml_diff>

<commit_message>
todos os executaveis funcionando
</commit_message>
<xml_diff>
--- a/cnpj.xlsx
+++ b/cnpj.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bruno.martins\Desktop\Sieg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D35007D3-EBAA-4974-A02A-C3B9C37A80CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4E52AB-4DBD-44B4-8666-F7F99C966DD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="181">
   <si>
     <t>CNPJ</t>
   </si>
@@ -33,6 +33,9 @@
     <t>05.574.628/0001-14</t>
   </si>
   <si>
+    <t>27.935.508/0001-38</t>
+  </si>
+  <si>
     <t>27.988.301/0001-21</t>
   </si>
   <si>
@@ -48,13 +51,523 @@
     <t>22.726.051/0001-38</t>
   </si>
   <si>
-    <t>27.935.508/0001-38</t>
-  </si>
-  <si>
     <t>34.467.517/0001-07</t>
   </si>
   <si>
     <t>46.701.113/0001-15</t>
+  </si>
+  <si>
+    <t>28.860.597/0001-63</t>
+  </si>
+  <si>
+    <t>42.856.348/0001-25</t>
+  </si>
+  <si>
+    <t>14.240.002/0001-62</t>
+  </si>
+  <si>
+    <t>02.573.131/0001-93</t>
+  </si>
+  <si>
+    <t>03.978.105/0001-08</t>
+  </si>
+  <si>
+    <t>34.127.889/0001-94</t>
+  </si>
+  <si>
+    <t>49.918.766/0001-49</t>
+  </si>
+  <si>
+    <t>51.335.694/0001-59</t>
+  </si>
+  <si>
+    <t>44.941.818/000-84</t>
+  </si>
+  <si>
+    <t>05.552.601/0001-20</t>
+  </si>
+  <si>
+    <t>15.180.317/0001-24</t>
+  </si>
+  <si>
+    <t>11.023.210/0001-11</t>
+  </si>
+  <si>
+    <t>17.936.365/0001-25</t>
+  </si>
+  <si>
+    <t>24.205.101/0001-67</t>
+  </si>
+  <si>
+    <t>27.468.267/0001-64</t>
+  </si>
+  <si>
+    <t>10.493.581/0001-02</t>
+  </si>
+  <si>
+    <t>51.904.027/0001-40</t>
+  </si>
+  <si>
+    <t>22.039.550/0001-57</t>
+  </si>
+  <si>
+    <t>53.117.601/0001-45</t>
+  </si>
+  <si>
+    <t>48.620.694/0001-96</t>
+  </si>
+  <si>
+    <t>32.192.180/0001-47</t>
+  </si>
+  <si>
+    <t>01.803.861/0001-70</t>
+  </si>
+  <si>
+    <t>45.551.512/0001-84</t>
+  </si>
+  <si>
+    <t>12.407.089/0001-94</t>
+  </si>
+  <si>
+    <t>49.920.531/0001-91</t>
+  </si>
+  <si>
+    <t>10.251.103/0001-88</t>
+  </si>
+  <si>
+    <t>04.591.902/0001-09</t>
+  </si>
+  <si>
+    <t>20.330.514/0001-12</t>
+  </si>
+  <si>
+    <t>05.426.225/0001-28</t>
+  </si>
+  <si>
+    <t>24.080.055/0001-17</t>
+  </si>
+  <si>
+    <t>53.858.320/0001-43</t>
+  </si>
+  <si>
+    <t>37.812.627/0001-57</t>
+  </si>
+  <si>
+    <t>45.528.148/0001-31</t>
+  </si>
+  <si>
+    <t>08.493.672/0001-98</t>
+  </si>
+  <si>
+    <t>57.190.544/0001-80</t>
+  </si>
+  <si>
+    <t>64.958.663/0001-04</t>
+  </si>
+  <si>
+    <t>31.253.286/0001-40</t>
+  </si>
+  <si>
+    <t>02.361.748/0001-45</t>
+  </si>
+  <si>
+    <t>19.221.171/0001-79</t>
+  </si>
+  <si>
+    <t>14.441.136/0001-41</t>
+  </si>
+  <si>
+    <t>17.161.602/0001-23</t>
+  </si>
+  <si>
+    <t>41.539.045/0001-16</t>
+  </si>
+  <si>
+    <t>11.819.159/0001-59</t>
+  </si>
+  <si>
+    <t>48.620.694/0002-77</t>
+  </si>
+  <si>
+    <t>49.920.531/0002-72</t>
+  </si>
+  <si>
+    <t>26.899.221/0003-07</t>
+  </si>
+  <si>
+    <t>10.493.581/0003-66</t>
+  </si>
+  <si>
+    <t>48.620.694/0003-58</t>
+  </si>
+  <si>
+    <t>12.407.089/0002-75</t>
+  </si>
+  <si>
+    <t>49.920.531/0003-53</t>
+  </si>
+  <si>
+    <t>57.622.722/0002-86</t>
+  </si>
+  <si>
+    <t>12.407.089/0003-56</t>
+  </si>
+  <si>
+    <t>49.920.531/0004-34</t>
+  </si>
+  <si>
+    <t>04.253.313/0003-74</t>
+  </si>
+  <si>
+    <t>04.253.313/0004-55</t>
+  </si>
+  <si>
+    <t>46.905.296/0001-90</t>
+  </si>
+  <si>
+    <t>45.551.512/0002-65</t>
+  </si>
+  <si>
+    <t>37.438.812/0001-23</t>
+  </si>
+  <si>
+    <t>13.216.823/0001-09</t>
+  </si>
+  <si>
+    <t>64.059.009/0001-50</t>
+  </si>
+  <si>
+    <t>09.241.535/0001-29</t>
+  </si>
+  <si>
+    <t>74.625.369/0001-26</t>
+  </si>
+  <si>
+    <t>14.003.724/0001-01</t>
+  </si>
+  <si>
+    <t>30.922.463/0001-71</t>
+  </si>
+  <si>
+    <t>13.871.662/0001-89</t>
+  </si>
+  <si>
+    <t>72.815.350/0001-17</t>
+  </si>
+  <si>
+    <t>01.083.122/0001-51</t>
+  </si>
+  <si>
+    <t>27.324.473/0001-09</t>
+  </si>
+  <si>
+    <t>37.650.866/0001-58</t>
+  </si>
+  <si>
+    <t>47.734.947/0001-90</t>
+  </si>
+  <si>
+    <t>32.707.447/0001-91</t>
+  </si>
+  <si>
+    <t>04.253.313/0001-02</t>
+  </si>
+  <si>
+    <t>18.101.284/0001-78</t>
+  </si>
+  <si>
+    <t>57.622.722/0001-03</t>
+  </si>
+  <si>
+    <t>09.142.005/0001-23</t>
+  </si>
+  <si>
+    <t>20.533.990/0001-30</t>
+  </si>
+  <si>
+    <t>10.350.863/0001-42</t>
+  </si>
+  <si>
+    <t>07.595.849/0001-02</t>
+  </si>
+  <si>
+    <t>43.849.534/0001-08</t>
+  </si>
+  <si>
+    <t>55.807.715/0001-42</t>
+  </si>
+  <si>
+    <t>20.667.541/0001-85</t>
+  </si>
+  <si>
+    <t>09.578.248/0001-09</t>
+  </si>
+  <si>
+    <t>23.857.176/0001-60</t>
+  </si>
+  <si>
+    <t>15.503.556/0001-78</t>
+  </si>
+  <si>
+    <t>20.901.766/0001-54</t>
+  </si>
+  <si>
+    <t>09.284.051/0001-67</t>
+  </si>
+  <si>
+    <t>42.177.591/0001-17</t>
+  </si>
+  <si>
+    <t>29.022.776/0001-94</t>
+  </si>
+  <si>
+    <t>02.316.330/0001-16</t>
+  </si>
+  <si>
+    <t>45.481.709/0001-94</t>
+  </si>
+  <si>
+    <t>02.344.159/0001-59</t>
+  </si>
+  <si>
+    <t>13.452.799/0001-07</t>
+  </si>
+  <si>
+    <t>05.350.981/0001-10</t>
+  </si>
+  <si>
+    <t>11.688.117/0001-26</t>
+  </si>
+  <si>
+    <t>08.059.154/0001-60</t>
+  </si>
+  <si>
+    <t>43.188.402/0001-74</t>
+  </si>
+  <si>
+    <t>23.343.042/0001-20</t>
+  </si>
+  <si>
+    <t>57.092.912/0001-58</t>
+  </si>
+  <si>
+    <t>46.747.455/0001-76</t>
+  </si>
+  <si>
+    <t>09.240.049/0001-96</t>
+  </si>
+  <si>
+    <t>09.419.898/0001-01</t>
+  </si>
+  <si>
+    <t>19.726.627/0001-52</t>
+  </si>
+  <si>
+    <t>41.319.486/0001-02</t>
+  </si>
+  <si>
+    <t>48.461.953/0001-83</t>
+  </si>
+  <si>
+    <t>18.583.562/0001-70</t>
+  </si>
+  <si>
+    <t>21.508.579/0001-78</t>
+  </si>
+  <si>
+    <t>10.779.535/0001-66</t>
+  </si>
+  <si>
+    <t>52.100.416/0001-85</t>
+  </si>
+  <si>
+    <t>11.850.406/0001-80</t>
+  </si>
+  <si>
+    <t>18.933.521/0001-67</t>
+  </si>
+  <si>
+    <t>03.409.583/0001-05</t>
+  </si>
+  <si>
+    <t>38.311.265/0001-83</t>
+  </si>
+  <si>
+    <t>02.961.049/0001-36</t>
+  </si>
+  <si>
+    <t>20.072.176/0001-66</t>
+  </si>
+  <si>
+    <t>52.490.938/0001-30</t>
+  </si>
+  <si>
+    <t>55.121.844/0001-82</t>
+  </si>
+  <si>
+    <t>04.494.585/0001-02</t>
+  </si>
+  <si>
+    <t>44.734.994/0001-45</t>
+  </si>
+  <si>
+    <t>07.499.258/0001-23</t>
+  </si>
+  <si>
+    <t>50.830.820/0001-89</t>
+  </si>
+  <si>
+    <t>10.265.831/0001-49</t>
+  </si>
+  <si>
+    <t>05.667.946/0001-20</t>
+  </si>
+  <si>
+    <t>09.550.876/0001-86</t>
+  </si>
+  <si>
+    <t>01.706.432/0001-85</t>
+  </si>
+  <si>
+    <t>33.863.050/0001-51</t>
+  </si>
+  <si>
+    <t>33.579.158/0001-17</t>
+  </si>
+  <si>
+    <t>46.472.550/0001-04</t>
+  </si>
+  <si>
+    <t>43.849.399/0001-92</t>
+  </si>
+  <si>
+    <t>00.162.337/0001-03</t>
+  </si>
+  <si>
+    <t>17.630.452/0001-50</t>
+  </si>
+  <si>
+    <t>68.210.665/0001-63</t>
+  </si>
+  <si>
+    <t>47.192.621/0001-88</t>
+  </si>
+  <si>
+    <t>10.798.563/0001-20</t>
+  </si>
+  <si>
+    <t>30.353.141/0001-59</t>
+  </si>
+  <si>
+    <t>07.153.849/0001-44</t>
+  </si>
+  <si>
+    <t>96.682.067/0001-22</t>
+  </si>
+  <si>
+    <t>06.956.200/0001-07</t>
+  </si>
+  <si>
+    <t>27.547.731/0001-08</t>
+  </si>
+  <si>
+    <t>16.550.677/0001-33</t>
+  </si>
+  <si>
+    <t>11.024.035/0001-87</t>
+  </si>
+  <si>
+    <t>22.812.385/0001-24</t>
+  </si>
+  <si>
+    <t>35.794.193/0001-84</t>
+  </si>
+  <si>
+    <t>00.574.215/0001-16</t>
+  </si>
+  <si>
+    <t>39.814.432/0001-71</t>
+  </si>
+  <si>
+    <t>19.761.898/0001-49</t>
+  </si>
+  <si>
+    <t>52.314.002/0001-59</t>
+  </si>
+  <si>
+    <t>29.933.257/0001-88</t>
+  </si>
+  <si>
+    <t>24.635.002/0001-15</t>
+  </si>
+  <si>
+    <t>00.183.296/0001-23</t>
+  </si>
+  <si>
+    <t>39.465.176/0001-54</t>
+  </si>
+  <si>
+    <t>08.732.024/0001-47</t>
+  </si>
+  <si>
+    <t>26.899.221/0001-37</t>
+  </si>
+  <si>
+    <t>74.638.834/0001-63</t>
+  </si>
+  <si>
+    <t>52.845.435/0001-30</t>
+  </si>
+  <si>
+    <t>40.129.573/0001-34</t>
+  </si>
+  <si>
+    <t>44.361.705/0001-00</t>
+  </si>
+  <si>
+    <t>11.685.846/0001-29</t>
+  </si>
+  <si>
+    <t>05.650.012/0001-85</t>
+  </si>
+  <si>
+    <t>55.424.291/0001-37</t>
+  </si>
+  <si>
+    <t>14.975.895/0001-94</t>
+  </si>
+  <si>
+    <t>04.581.091/0001-57</t>
+  </si>
+  <si>
+    <t>02.458.761/0001-17</t>
+  </si>
+  <si>
+    <t>11.737.802/0001-03</t>
+  </si>
+  <si>
+    <t>51.307.276/0001-58</t>
+  </si>
+  <si>
+    <t>43.750.941/0001-55</t>
+  </si>
+  <si>
+    <t>54.898.865/0001-46</t>
+  </si>
+  <si>
+    <t>07.538.935/0001-75</t>
+  </si>
+  <si>
+    <t>19.956.967/0001-70</t>
+  </si>
+  <si>
+    <t>48.869.875/0001-50</t>
+  </si>
+  <si>
+    <t>31.532.172/0001-30</t>
+  </si>
+  <si>
+    <t>01.054.712/0001-56</t>
   </si>
 </sst>
 </file>
@@ -383,8 +896,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A181"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
+      <selection activeCell="A129" sqref="A129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,7 +912,7 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -409,27 +922,27 @@
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
@@ -443,517 +956,859 @@
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+      <c r="A23" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
+      <c r="A34" s="1" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+      <c r="A36" s="1" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+      <c r="A37" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
+      <c r="A38" s="1" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
+      <c r="A39" s="1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
+      <c r="A40" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+      <c r="A41" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
+      <c r="A42" s="1" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
+      <c r="A43" s="1" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
+      <c r="A44" s="1" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
+      <c r="A45" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
+      <c r="A48" s="1" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
+      <c r="A49" s="1" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
+      <c r="A50" s="1" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
+      <c r="A51" s="1" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
+      <c r="A52" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
+      <c r="A53" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="1"/>
+      <c r="A54" s="1" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
+      <c r="A55" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="1"/>
+      <c r="A56" s="1" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
+      <c r="A57" s="1" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
+      <c r="A58" s="1" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
+      <c r="A59" s="1" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
+      <c r="A60" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
+      <c r="A61" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
+      <c r="A62" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
+      <c r="A63" s="1" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="64" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
+      <c r="A64" s="1" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
+      <c r="A65" s="1" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
+      <c r="A66" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
+      <c r="A67" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
+      <c r="A68" s="1" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1"/>
+      <c r="A69" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1"/>
+      <c r="A70" s="1" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1"/>
+      <c r="A71" s="1" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A72" s="1"/>
+      <c r="A72" s="1" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="1"/>
+      <c r="A73" s="1" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A74" s="1"/>
+      <c r="A74" s="1" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="1"/>
+      <c r="A75" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A76" s="1"/>
+      <c r="A76" s="1" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="1"/>
+      <c r="A77" s="1" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A78" s="1"/>
+      <c r="A78" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="1"/>
+      <c r="A79" s="1" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A80" s="1"/>
+      <c r="A80" s="1" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="1"/>
+      <c r="A81" s="1" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="1"/>
+      <c r="A82" s="1" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="1"/>
+      <c r="A83" s="1" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="1"/>
+      <c r="A84" s="1" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="1"/>
+      <c r="A85" s="1" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="1"/>
+      <c r="A86" s="1" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="1"/>
+      <c r="A87" s="1" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="1"/>
+      <c r="A88" s="1" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="1"/>
+      <c r="A89" s="1" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="1"/>
+      <c r="A90" s="1" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="1"/>
+      <c r="A91" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="1"/>
+      <c r="A92" s="1" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="1"/>
+      <c r="A93" s="1" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="1"/>
+      <c r="A94" s="1" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="1"/>
+      <c r="A95" s="1" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="1"/>
+      <c r="A96" s="1" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="1"/>
+      <c r="A97" s="1" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="1"/>
+      <c r="A98" s="1" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
+      <c r="A99" s="1" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="1"/>
+      <c r="A100" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="1"/>
+      <c r="A101" s="1" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="1"/>
+      <c r="A102" s="1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="1"/>
+      <c r="A103" s="1" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="1"/>
+      <c r="A104" s="1" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="1"/>
+      <c r="A105" s="1" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="1"/>
+      <c r="A106" s="1" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="1"/>
+      <c r="A107" s="1" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="1"/>
+      <c r="A108" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="1"/>
+      <c r="A109" s="1" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="1"/>
+      <c r="A110" s="1" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="1"/>
+      <c r="A111" s="1" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="1"/>
+      <c r="A112" s="1" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="1"/>
+      <c r="A113" s="1" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="1"/>
+      <c r="A114" s="1" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="1"/>
+      <c r="A115" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="1"/>
+      <c r="A116" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="1"/>
+      <c r="A117" s="1" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="1"/>
+      <c r="A118" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="1"/>
+      <c r="A119" s="1" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="1"/>
+      <c r="A120" s="1" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="1"/>
+      <c r="A121" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
+      <c r="A122" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
+      <c r="A123" s="1" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
+      <c r="A124" s="1" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="1"/>
+      <c r="A125" s="1" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
+      <c r="A126" s="1" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="1"/>
+      <c r="A127" s="1" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="1"/>
+      <c r="A128" s="1" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="1"/>
+      <c r="A129" s="1" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="1"/>
+      <c r="A130" s="1" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="1"/>
+      <c r="A131" s="1" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="1"/>
+      <c r="A132" s="1" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="1"/>
+      <c r="A133" s="1" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="1"/>
+      <c r="A134" s="1" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="1"/>
+      <c r="A135" s="1" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="1"/>
+      <c r="A136" s="1" t="s">
+        <v>135</v>
+      </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
+      <c r="A137" s="1" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1"/>
+      <c r="A138" s="1" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="1"/>
+      <c r="A139" s="1" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="1"/>
+      <c r="A140" s="1" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="1"/>
+      <c r="A141" s="1" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="1"/>
+      <c r="A142" s="1" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="1"/>
+      <c r="A143" s="1" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="1"/>
+      <c r="A144" s="1" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="1"/>
+      <c r="A145" s="1" t="s">
+        <v>144</v>
+      </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="1"/>
+      <c r="A146" s="1" t="s">
+        <v>145</v>
+      </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="1"/>
+      <c r="A147" s="1" t="s">
+        <v>146</v>
+      </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="1"/>
+      <c r="A148" s="1" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="1"/>
+      <c r="A149" s="1" t="s">
+        <v>148</v>
+      </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="1"/>
+      <c r="A150" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="1"/>
+      <c r="A151" s="1" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="1"/>
+      <c r="A152" s="1" t="s">
+        <v>151</v>
+      </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="1"/>
+      <c r="A153" s="1" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="1"/>
+      <c r="A154" s="1" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="1"/>
+      <c r="A155" s="1" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="1"/>
+      <c r="A156" s="1" t="s">
+        <v>155</v>
+      </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="1"/>
+      <c r="A157" s="1" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="1"/>
+      <c r="A158" s="1" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="1"/>
+      <c r="A159" s="1" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="1"/>
+      <c r="A160" s="1" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="1"/>
+      <c r="A161" s="1" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="1"/>
+      <c r="A162" s="1" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="1"/>
+      <c r="A163" s="1" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="1"/>
+      <c r="A164" s="1" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="1"/>
+      <c r="A165" s="1" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A166" s="1"/>
+      <c r="A166" s="1" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A167" s="1"/>
+      <c r="A167" s="1" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A168" s="1"/>
+      <c r="A168" s="1" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A169" s="1"/>
+      <c r="A169" s="1" t="s">
+        <v>168</v>
+      </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A170" s="1"/>
+      <c r="A170" s="1" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A171" s="1"/>
+      <c r="A171" s="1" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A172" s="1"/>
+      <c r="A172" s="1" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A173" s="1"/>
+      <c r="A173" s="1" t="s">
+        <v>172</v>
+      </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A174" s="1"/>
+      <c r="A174" s="1" t="s">
+        <v>173</v>
+      </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A175" s="1"/>
+      <c r="A175" s="1" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A176" s="1"/>
+      <c r="A176" s="1" t="s">
+        <v>175</v>
+      </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A177" s="1"/>
+      <c r="A177" s="1" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A178" s="1"/>
+      <c r="A178" s="1" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A179" s="1"/>
+      <c r="A179" s="1" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="180" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A180" s="1"/>
+      <c r="A180" s="1" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A181" s="1"/>
+      <c r="A181" s="1" t="s">
+        <v>180</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>